<commit_message>
Removed all Hard Coding. Did use of Apache POI and used Environment Class.
</commit_message>
<xml_diff>
--- a/AutomaticResumeFilter/src/main/LoginDetails.xlsx
+++ b/AutomaticResumeFilter/src/main/LoginDetails.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yashmittal2\Desktop\Automatic-Resume-Filter-Automation\AutomaticResumeFilter\src\main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83BEF80E-CFA5-4C49-9E4A-C509C7DD64B3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7152D3B7-FDCC-4F46-8956-33F4387BD8EC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>Username</t>
   </si>
@@ -40,6 +41,15 @@
   </si>
   <si>
     <t>yyashmittal@gmail.com</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>expert123</t>
   </si>
 </sst>
 </file>
@@ -69,12 +79,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -90,9 +106,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -376,8 +393,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -388,13 +405,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -417,4 +434,40 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{236DB4D4-3FB3-483A-B120-D161C3065862}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="11.90625" customWidth="1"/>
+    <col min="2" max="2" width="15.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Done with Extent report.
</commit_message>
<xml_diff>
--- a/AutomaticResumeFilter/src/main/LoginDetails.xlsx
+++ b/AutomaticResumeFilter/src/main/LoginDetails.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yashmittal2\Desktop\Automatic-Resume-Filter-Automation\AutomaticResumeFilter\src\main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7152D3B7-FDCC-4F46-8956-33F4387BD8EC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E1D1A52-20A8-4C08-B2B9-90BA53877007}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,7 +49,7 @@
     <t>password</t>
   </si>
   <si>
-    <t>expert123</t>
+    <t>qwer1234</t>
   </si>
 </sst>
 </file>
@@ -441,7 +441,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>